<commit_message>
Updated Triangles-Design.pdf to more accuretly reflect design.
</commit_message>
<xml_diff>
--- a/Error-Checking.xlsx
+++ b/Error-Checking.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
   <si>
     <t>Test Case</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Test Suite/Class</t>
   </si>
   <si>
-    <t>double diffY = m_point2-&gt;getY() - m_point1-&gt;getX();</t>
-  </si>
-  <si>
     <t>#1</t>
   </si>
   <si>
@@ -53,13 +50,6 @@
     <t>should be</t>
   </si>
   <si>
-    <t>return isValid() &amp;&amp;
-           otherEdge.isValid() &amp;&amp;
-           areSlopesEquivalent(getSlopeX(), otherEdge.getSlopeX()) &amp;&amp;
-           areSlopesEquivalent(getSlopeY(), otherEdge.getSlopeY()) &amp;&amp;
-           areSlopesEquivalent(getSlopeZ(), otherEdge.getSlopeX());</t>
-  </si>
-  <si>
     <t>#2</t>
   </si>
   <si>
@@ -70,7 +60,133 @@
   </si>
   <si>
     <r>
-      <t>return (isValid() &amp;&amp;
+      <t>double diffY = m_point2-&gt;getY() - m_point1-&gt;get</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>();</t>
+    </r>
+  </si>
+  <si>
+    <t>Edge::isParrallelTo</t>
+  </si>
+  <si>
+    <t>Edge::getLength</t>
+  </si>
+  <si>
+    <t>Point::isEquivalentTo</t>
+  </si>
+  <si>
+    <t>comparing a point to itself</t>
+  </si>
+  <si>
+    <t>returns false when should return true</t>
+  </si>
+  <si>
+    <t>Point::initialize</t>
+  </si>
+  <si>
+    <t>#4</t>
+  </si>
+  <si>
+    <t>#3</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>#6</t>
+  </si>
+  <si>
+    <r>
+      <t>m_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = convertStringToDouble(values[2], &amp;m_valid);</t>
+    </r>
+  </si>
+  <si>
+    <t>Point::checkForInfinity</t>
+  </si>
+  <si>
+    <t>makes sure no values are set to Inifinity</t>
+  </si>
+  <si>
+    <t>m_z was set to be true if equal to infinity</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">m_valid = (m_x != INFINITY &amp;&amp; m_y != INFINITY &amp;&amp; m_z </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= INFINITY);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">return </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>isValid() &amp;&amp;
            otherEdge.isValid() &amp;&amp;
            areSlopesEquivalent(getSlopeX(), otherEdge.getSlopeX()) &amp;&amp;
            areSlopesEquivalent(getSlopeY(), otherEdge.getSlopeY()) &amp;&amp;
@@ -92,7 +208,365 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>()));</t>
+      <t>())</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>Failure in e.getSlopeZ(), slope=inf (expecting 0)
+Execute EdgeTester::testEdge02
+Failure in e.getSlopeZ(), slope=inf (expecting 1.118033989)</t>
+  </si>
+  <si>
+    <t>EdgeTester::testEdge01</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">if (xyOffset </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= 0)</t>
+    </r>
+  </si>
+  <si>
+    <t>checking that the slope is valid</t>
+  </si>
+  <si>
+    <t>double Edge::getSlopeZ() const</t>
+  </si>
+  <si>
+    <r>
+      <t>m_points[2] = new Point(values[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]);</t>
+    </r>
+  </si>
+  <si>
+    <t>Triangle::Triangle(std::string&amp; triangleStr)</t>
+  </si>
+  <si>
+    <t>Triangle: unexpected type of N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TriangleTester::testConstructorWithStrings
+</t>
+  </si>
+  <si>
+    <t>#7</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">double s = ( a + b + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)/2;</t>
+    </r>
+  </si>
+  <si>
+    <t>Triangle::computerArea()</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(approximatelyEquals(a, b, m_edgeLengthThreshold) ||
+                    approximatelyEquals(b, c, m_edgeLengthThreshold) ||
+                    approximatelyEquals(c, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, m_edgeLengthThreshold))</t>
+    </r>
+  </si>
+  <si>
+    <t>char Triangle::getTriangleType() const</t>
+  </si>
+  <si>
+    <r>
+      <t>if (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>isTriangle())</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>isTriangle())</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(approximatelyEquals(a, b, m_edgeLengthThreshold) ||
+                    approximatelyEquals(b, c, m_edgeLengthThreshold) ||
+                    approximatelyEquals(c, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, m_edgeLengthThreshold))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">double s = ( a + b + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)/2;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>m_points[2] = new Point(values[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">if (xyOffset </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= 0)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">m_valid = (m_x != INFINITY &amp;&amp; m_y != INFINITY &amp;&amp; m_z </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= INFINITY);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>m_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = convertStringToDouble(values[2], &amp;m_valid);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>return isValid() &amp;&amp;
+           otherEdge.isValid() &amp;&amp;
+           areSlopesEquivalent(getSlopeX(), otherEdge.getSlopeX()) &amp;&amp;
+           areSlopesEquivalent(getSlopeY(), otherEdge.getSlopeY()) &amp;&amp;
+           areSlopesEquivalent(getSlopeZ(), otherEdge.getSlope</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>());</t>
     </r>
   </si>
   <si>
@@ -105,7 +579,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>Y</t>
+      <t>X</t>
     </r>
     <r>
       <rPr>
@@ -119,60 +593,126 @@
     </r>
   </si>
   <si>
-    <t>Edge::isParrallelTo</t>
-  </si>
-  <si>
-    <t>Edge::getLength</t>
-  </si>
-  <si>
-    <t>Point::isEquivalentTo</t>
-  </si>
-  <si>
-    <t>comparing a point to itself</t>
-  </si>
-  <si>
-    <t>returns false when should return true</t>
-  </si>
-  <si>
-    <t>Point::initialize</t>
-  </si>
-  <si>
-    <t>#4</t>
-  </si>
-  <si>
-    <t>#3</t>
-  </si>
-  <si>
-    <t>#5</t>
-  </si>
-  <si>
-    <t>#6</t>
-  </si>
-  <si>
-    <t>m_y = convertStringToDouble(values[2], &amp;m_valid);</t>
-  </si>
-  <si>
-    <r>
-      <t>m_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>z</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = convertStringToDouble(values[2], &amp;m_valid);</t>
-    </r>
+    <t>#7,8,9,10</t>
+  </si>
+  <si>
+    <t>#8</t>
+  </si>
+  <si>
+    <t>#9</t>
+  </si>
+  <si>
+    <t>#10</t>
+  </si>
+  <si>
+    <t>#11</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">return edge.getLength() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> m_minDistance;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">return edge.getLength() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> m_minDistance;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>std::cout &lt;&lt; "Execute TriangleTester::test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>First</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Constructor" &lt;&lt; std::endl;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>std::cout &lt;&lt; "Execute TriangleTester::test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>ConstructorWithStrings</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" &lt;&lt; std::endl;</t>
+    </r>
+  </si>
+  <si>
+    <t>TriangleTester::testFirstConstructor</t>
+  </si>
+  <si>
+    <t>cout statement did not reflect the proper function name being tested</t>
+  </si>
+  <si>
+    <t>see other table</t>
+  </si>
+  <si>
+    <t>check that the constructor for strings is working</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -330,7 +870,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -346,6 +886,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,22 +1173,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I24"/>
+  <dimension ref="B1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="3" max="3" width="34.1640625" customWidth="1"/>
+    <col min="4" max="4" width="57.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.5" customWidth="1"/>
-    <col min="7" max="7" width="56" customWidth="1"/>
-    <col min="8" max="8" width="59" customWidth="1"/>
-    <col min="9" max="9" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="65.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="59.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -658,69 +1208,109 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="D3" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="E3" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
+      <c r="D4" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="E4" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9" t="s">
+    </row>
+    <row r="8" spans="2:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="B8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
+    <row r="9" spans="2:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B9" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="B10" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="10"/>
@@ -766,76 +1356,158 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="G18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="7" t="s">
-        <v>7</v>
-      </c>
       <c r="I18" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F19" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="I19" s="5"/>
     </row>
     <row r="20" spans="2:9" ht="80" x14ac:dyDescent="0.2">
       <c r="F20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F21" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I21" s="5"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F22" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F23" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23" s="5"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F25" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F26" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="F27" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F28" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I29" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>